<commit_message>
Add mul_lin_reg.power_transform with basic testing
Also update TestModelReduction to import Data in the proper format. Known issue: mul_lin_reg.power_transform.Box_Cox_transform does not have lambda2
</commit_message>
<xml_diff>
--- a/tests/functions/mult_lin_reg_utils/Data.xlsx
+++ b/tests/functions/mult_lin_reg_utils/Data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\tests\functions\mult_lin_reg_utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01BB364-FA4D-4955-AC12-506219EA7CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2125251-4A72-4E2C-A03C-5ACC88FE19FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="6" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
     <sheet name="Design Parameters" sheetId="1" r:id="rId2"/>
     <sheet name="Responses" sheetId="3" r:id="rId3"/>
     <sheet name="Other Parameters" sheetId="4" r:id="rId4"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Features</t>
   </si>
@@ -105,6 +105,9 @@
     <t>Code</t>
   </si>
   <si>
+    <t>Run</t>
+  </si>
+  <si>
     <t>Roll temperature (°C)</t>
   </si>
   <si>
@@ -163,12 +166,6 @@
   </si>
   <si>
     <t>Not applicable</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
   </si>
 </sst>
 </file>
@@ -199,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -207,26 +204,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,8 +225,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,340 +592,398 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E0361B-3562-4DFE-9BED-FB5013454095}">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2412BF-878C-45DB-8461-781C8212B1FA}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>85</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D2" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="E2">
+        <v>161.26647034381304</v>
+      </c>
+      <c r="F2">
+        <v>72.041289257868158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>85</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D3" s="7">
+        <v>33.83</v>
+      </c>
+      <c r="E3">
+        <v>163.24631274749157</v>
+      </c>
+      <c r="F3">
+        <v>85.186684022091868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" s="7">
+        <v>85</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D4" s="7">
+        <v>28.22</v>
+      </c>
+      <c r="E4">
+        <v>163.61126514902989</v>
+      </c>
+      <c r="F4">
+        <v>89.828855429747492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B5" s="7">
+        <v>120</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D5" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="E5">
+        <v>162.54669346536949</v>
+      </c>
+      <c r="F5">
+        <v>59.174622450856383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0.906667</v>
-      </c>
-      <c r="D2" s="6">
-        <v>161.26647</v>
-      </c>
-      <c r="E2" s="6">
-        <v>72.041289000000006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B3" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C3" s="6">
-        <v>-2.8333000000000001E-2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>163.24631299999999</v>
-      </c>
-      <c r="E3" s="6">
-        <v>85.186684</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>-0.96333299999999999</v>
-      </c>
-      <c r="D4" s="6">
-        <v>163.611265</v>
-      </c>
-      <c r="E4" s="6">
-        <v>89.828855000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>0.16666700000000001</v>
-      </c>
-      <c r="B5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0.906667</v>
-      </c>
-      <c r="D5" s="6">
-        <v>162.546693</v>
-      </c>
-      <c r="E5" s="6">
-        <v>59.174621999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>0.16666700000000001</v>
-      </c>
-      <c r="B6" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C6" s="6">
-        <v>-2.8333000000000001E-2</v>
-      </c>
-      <c r="D6" s="6">
-        <v>163.13595100000001</v>
-      </c>
-      <c r="E6" s="6">
-        <v>81.773995999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>0.16666700000000001</v>
-      </c>
-      <c r="B7" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>-0.96333299999999999</v>
-      </c>
-      <c r="D7" s="6">
-        <v>162.57257200000001</v>
-      </c>
-      <c r="E7" s="6">
-        <v>84.951190999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.906667</v>
-      </c>
-      <c r="D8" s="6">
-        <v>160.603309</v>
-      </c>
-      <c r="E8" s="6">
-        <v>30.733031</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
-      <c r="B9" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C9" s="6">
-        <v>-2.8333000000000001E-2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>161.72268600000001</v>
-      </c>
-      <c r="E9" s="6">
-        <v>84.945757999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C10" s="6">
-        <v>-0.96333299999999999</v>
-      </c>
-      <c r="D10" s="6">
-        <v>162.29596900000001</v>
-      </c>
-      <c r="E10" s="6">
-        <v>69.421891000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.906667</v>
-      </c>
-      <c r="D11" s="6">
-        <v>160.39388400000001</v>
-      </c>
-      <c r="E11" s="6">
-        <v>8.8999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6">
-        <v>-2.8333000000000001E-2</v>
-      </c>
-      <c r="D12" s="6">
-        <v>162.23912799999999</v>
-      </c>
-      <c r="E12" s="6">
-        <v>21.63635</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6">
-        <v>-0.96333299999999999</v>
-      </c>
-      <c r="D13" s="6">
-        <v>162.16754499999999</v>
-      </c>
-      <c r="E13" s="6">
-        <v>11.601307</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
-        <v>0.16666700000000001</v>
-      </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.906667</v>
-      </c>
-      <c r="D14" s="6">
-        <v>161.66590500000001</v>
-      </c>
-      <c r="E14" s="6">
-        <v>3.49661</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
-        <v>0.16666700000000001</v>
-      </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6">
-        <v>-2.8333000000000001E-2</v>
-      </c>
-      <c r="D15" s="6">
-        <v>161.94140300000001</v>
-      </c>
-      <c r="E15" s="6">
-        <v>17.198715</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
-        <v>0.16666700000000001</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6">
-        <v>-0.96333299999999999</v>
-      </c>
-      <c r="D16" s="6">
-        <v>162.80112399999999</v>
-      </c>
-      <c r="E16" s="6">
-        <v>14.892531</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.906667</v>
-      </c>
-      <c r="D17" s="6">
-        <v>160.75407999999999</v>
-      </c>
-      <c r="E17" s="6">
-        <v>8.92E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
-        <v>1</v>
-      </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6">
-        <v>-2.8333000000000001E-2</v>
-      </c>
-      <c r="D18" s="6">
-        <v>161.73769999999999</v>
-      </c>
-      <c r="E18" s="6">
-        <v>15.862730000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="6">
-        <v>-0.96333299999999999</v>
-      </c>
-      <c r="D19" s="6">
-        <v>162.06572600000001</v>
-      </c>
-      <c r="E19" s="6">
-        <v>11.623512</v>
+      <c r="B6" s="7">
+        <v>120</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D6" s="7">
+        <v>33.83</v>
+      </c>
+      <c r="E6">
+        <v>163.13595123364951</v>
+      </c>
+      <c r="F6">
+        <v>81.773996381057302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>120</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D7" s="7">
+        <v>28.22</v>
+      </c>
+      <c r="E7">
+        <v>162.57257207035542</v>
+      </c>
+      <c r="F7">
+        <v>84.951190961672879</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>145</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D8" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="E8">
+        <v>160.60330891119415</v>
+      </c>
+      <c r="F8">
+        <v>30.733031121982521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>145</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D9" s="7">
+        <v>33.83</v>
+      </c>
+      <c r="E9">
+        <v>161.72268604850387</v>
+      </c>
+      <c r="F9">
+        <v>84.945758440531378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7">
+        <v>145</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="D10" s="7">
+        <v>28.22</v>
+      </c>
+      <c r="E10">
+        <v>162.29596943809688</v>
+      </c>
+      <c r="F10">
+        <v>69.421891154692503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>85</v>
+      </c>
+      <c r="C11" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="E11">
+        <v>160.39388420675371</v>
+      </c>
+      <c r="F11">
+        <v>8.8965527938430003E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <v>85</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>33.83</v>
+      </c>
+      <c r="E12">
+        <v>162.23912776090114</v>
+      </c>
+      <c r="F12">
+        <v>21.636350153652174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7">
+        <v>85</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D13" s="7">
+        <v>28.22</v>
+      </c>
+      <c r="E13">
+        <v>162.16754539251556</v>
+      </c>
+      <c r="F13">
+        <v>11.601307424285451</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>120</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D14" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="E14">
+        <v>161.66590458807934</v>
+      </c>
+      <c r="F14">
+        <v>3.4966099123584069</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>120</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D15" s="7">
+        <v>33.83</v>
+      </c>
+      <c r="E15">
+        <v>161.94140267693186</v>
+      </c>
+      <c r="F15">
+        <v>17.198715402852347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7">
+        <v>120</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D16" s="7">
+        <v>28.22</v>
+      </c>
+      <c r="E16">
+        <v>162.80112356445107</v>
+      </c>
+      <c r="F16">
+        <v>14.892530662050966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
+        <v>145</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>39.44</v>
+      </c>
+      <c r="E17">
+        <v>160.75407959775919</v>
+      </c>
+      <c r="F17">
+        <v>8.9214094531340604E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7">
+        <v>145</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D18" s="7">
+        <v>33.83</v>
+      </c>
+      <c r="E18">
+        <v>161.73770048700803</v>
+      </c>
+      <c r="F18">
+        <v>15.862730271587914</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7">
+        <v>145</v>
+      </c>
+      <c r="C19" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>28.22</v>
+      </c>
+      <c r="E19">
+        <v>162.06572573839108</v>
+      </c>
+      <c r="F19">
+        <v>11.623511691296509</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -976,10 +1019,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -987,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>85</v>
@@ -996,10 +1039,10 @@
         <v>145</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1007,7 +1050,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>2.7</v>
@@ -1016,10 +1059,10 @@
         <v>3.2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1027,7 +1070,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>28</v>
@@ -1036,10 +1079,10 @@
         <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1074,35 +1117,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1132,26 +1175,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>